<commit_message>
feat: finished the student management function of teacher
</commit_message>
<xml_diff>
--- a/ui/static/uploads/学生模板.xlsx
+++ b/ui/static/uploads/学生模板.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Git\GDUTMeow\MentalArithmeticApp\ui\static\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GamerNoTitle\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{328C1270-FC11-46DA-A50D-F8A057B721A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55329940-1DF9-43CC-8BC0-5ED048FCC974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{09AEBA47-B3A6-4150-9DFF-CAF74C8A7EB5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>学号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,14 @@
   </si>
   <si>
     <t>说明：1、学生的学号应该为学校的标准学号，即3xxx00xxxx的格式；2、学生的姓名根据中华人民共和国公安部的有关规定，不得大于15个汉字；3、学生的班级长度不得大于10个汉字；4、导入前您应该把示例数据删除，并加入自己的学生数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>00000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -121,12 +129,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,19 +473,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C44CAA-4F6F-4803-9110-45C269AD8B33}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,8 +496,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>3124004598</v>
       </c>
@@ -495,16 +510,19 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3224008517</v>
       </c>
@@ -514,14 +532,17 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3123005871</v>
       </c>
@@ -531,64 +552,67 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E5" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E6" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E7" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E8" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E9" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E10" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E2:J10"/>
+    <mergeCell ref="F2:K10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>